<commit_message>
Updated RiskAssessment.xlsx with new risks that were discovered during the project
</commit_message>
<xml_diff>
--- a/documentation/RiskAssessment.xlsx
+++ b/documentation/RiskAssessment.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25227"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="70" documentId="11_E60897F41BE170836B02CE998F75CCDC64E183C8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{790ABAF3-D2CB-4025-967B-89D24BAB8D46}"/>
+  <xr:revisionPtr revIDLastSave="124" documentId="11_E60897F41BE170836B02CE998F75CCDC64E183C8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{048BE40B-1272-402F-951C-6C0D6AE79B44}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="73">
   <si>
     <t>Risk Matrices</t>
   </si>
@@ -310,6 +310,30 @@
 and keep my work saved in multiple
 secure locations to decrease the
 Likelihood of loosing all of my work.</t>
+  </si>
+  <si>
+    <t>Getting aches</t>
+  </si>
+  <si>
+    <t>Getting aches can result in reduces productivity making my workflow less efficient</t>
+  </si>
+  <si>
+    <t>Ensure to take regular breaks, stretch and keep a good posture while working on the computer</t>
+  </si>
+  <si>
+    <t>Reagularly stretch and maintain a good posture while working</t>
+  </si>
+  <si>
+    <t>Getting Distracted</t>
+  </si>
+  <si>
+    <t>Getting distracted can reduce productivity and cause you to lose your train of thought</t>
+  </si>
+  <si>
+    <t>Ensure to keep my phone away from my workspace and wear headphones to reduce the chances of being distracted by occurrances in my surroundings</t>
+  </si>
+  <si>
+    <t>Create a work focus mode in my phone that only allows important notifications to come through when in work hours. Also create a seperate desktop on my pc to allow a disconnect between work and leisure, to ensure I'm not distracted and that I can take healthy breaks from work out of hours.</t>
   </si>
 </sst>
 </file>
@@ -393,7 +417,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -424,6 +448,15 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
@@ -740,10 +773,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J22"/>
+  <dimension ref="A1:J24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="H26" sqref="H26"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="31.28515625" defaultRowHeight="15"/>
@@ -1257,6 +1290,58 @@
       </c>
       <c r="J22" s="1"/>
     </row>
+    <row r="23" spans="1:10" ht="60.75">
+      <c r="B23" s="16" t="s">
+        <v>65</v>
+      </c>
+      <c r="C23" s="17" t="s">
+        <v>66</v>
+      </c>
+      <c r="D23" s="17" t="s">
+        <v>67</v>
+      </c>
+      <c r="E23" s="17" t="s">
+        <v>68</v>
+      </c>
+      <c r="F23" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="G23" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="H23" s="13">
+        <v>3</v>
+      </c>
+      <c r="I23" s="18">
+        <v>44687</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" ht="120" customHeight="1">
+      <c r="B24" s="16" t="s">
+        <v>69</v>
+      </c>
+      <c r="C24" s="17" t="s">
+        <v>70</v>
+      </c>
+      <c r="D24" s="17" t="s">
+        <v>71</v>
+      </c>
+      <c r="E24" s="17" t="s">
+        <v>72</v>
+      </c>
+      <c r="F24" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="G24" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="H24" s="13">
+        <v>4</v>
+      </c>
+      <c r="I24" s="18">
+        <v>44687</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>